<commit_message>
Small fixes and cleanup
</commit_message>
<xml_diff>
--- a/TEAM_Example/Team_Example_Challenge2/metrics/hackathon_final_scores.xlsx
+++ b/TEAM_Example/Team_Example_Challenge2/metrics/hackathon_final_scores.xlsx
@@ -568,7 +568,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TEAM_Diagnobac_Challenge2</t>
+          <t>TEAM_Example_Challenge2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -596,7 +596,7 @@
         <v>0.5346402</v>
       </c>
       <c r="J2" t="n">
-        <v>100</v>
+        <v>37.5</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -623,7 +623,7 @@
         <v>4.692804000000001</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T2" t="n">
         <v>7.070426666666666</v>
@@ -632,22 +632,18 @@
         <v>4.692804000000001</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W2" t="n">
-        <v>5.1808168</v>
+        <v>6.7808168</v>
       </c>
       <c r="X2" t="n">
-        <v>51.80816799999999</v>
+        <v>67.80816799999999</v>
       </c>
       <c r="Y2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>CDR3 identity &gt;= 95 percent</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>